<commit_message>
added ideas to design
</commit_message>
<xml_diff>
--- a/template_sheet.xlsx
+++ b/template_sheet.xlsx
@@ -402,16 +402,16 @@
         </is>
       </c>
       <c r="C2">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F2">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
@@ -426,16 +426,16 @@
         </is>
       </c>
       <c r="C3">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="E3">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F3">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
@@ -450,16 +450,16 @@
         </is>
       </c>
       <c r="C4">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E4">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -474,16 +474,16 @@
         </is>
       </c>
       <c r="C5">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E5">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -543,16 +543,16 @@
         </is>
       </c>
       <c r="C2">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D2">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F2">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
@@ -567,16 +567,16 @@
         </is>
       </c>
       <c r="C3">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E3">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
@@ -591,16 +591,16 @@
         </is>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D4">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F4">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
@@ -615,16 +615,16 @@
         </is>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D5">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E5">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F5">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>